<commit_message>
amended mapping, example and profile for zib FluidBalance after feedback
</commit_message>
<xml_diff>
--- a/Mappings/FluidBalance - STU3.xlsx
+++ b/Mappings/FluidBalance - STU3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="137">
   <si>
     <t>Subject</t>
   </si>
@@ -788,7 +788,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -829,7 +829,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -870,7 +870,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3801,7 +3801,7 @@
   <dimension ref="B2:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3977,7 +3977,9 @@
       <c r="P5" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="Q5" s="14"/>
+      <c r="Q5" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="R5" s="14"/>
       <c r="S5" s="2" t="s">
         <v>116</v>
@@ -4018,7 +4020,9 @@
       <c r="P6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="Q6" s="14"/>
+      <c r="Q6" s="14" t="s">
+        <v>117</v>
+      </c>
       <c r="R6" s="14"/>
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
@@ -4156,6 +4160,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -4346,22 +4365,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA1F4FB-A6CE-4AAF-8EB2-21729483ED50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{074CF55D-C3B1-4AF2-905A-ED84E325F4F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6E7AE7-456E-4C93-AAE7-62D72B615836}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4378,21 +4399,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{074CF55D-C3B1-4AF2-905A-ED84E325F4F0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACA1F4FB-A6CE-4AAF-8EB2-21729483ED50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>